<commit_message>
Data quality tables and cleaning up
</commit_message>
<xml_diff>
--- a/datasets/intermediate/Ghandour-2019-Fig1.xlsx
+++ b/datasets/intermediate/Ghandour-2019-Fig1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\HRTL-2016-2022\datasets\intermediate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8A740C-EEE8-447A-9A93-9B8B5688AEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A08C74F-40FB-49B8-B1EA-53A50CD973D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23085" yWindow="1125" windowWidth="22950" windowHeight="15345" xr2:uid="{0C469A4B-AC51-4451-A44C-76ABBC72F511}"/>
   </bookViews>
@@ -50,16 +50,16 @@
     <t>Physical Health and Motor Development</t>
   </si>
   <si>
-    <t>at_risk_G19</t>
-  </si>
-  <si>
-    <t>needs_support_G19</t>
-  </si>
-  <si>
-    <t>on_track_G19</t>
-  </si>
-  <si>
     <t>domain_2016</t>
+  </si>
+  <si>
+    <t>at_risk</t>
+  </si>
+  <si>
+    <t>needs_support</t>
+  </si>
+  <si>
+    <t>on_track</t>
   </si>
 </sst>
 </file>
@@ -443,23 +443,23 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>